<commit_message>
fix in column names spaces and name
</commit_message>
<xml_diff>
--- a/Data/riket2023_åk9_np.xlsx
+++ b/Data/riket2023_åk9_np.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Engelska"/>
@@ -144,7 +144,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +157,12 @@
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -175,7 +181,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -218,28 +224,28 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -962,6 +968,336 @@
   </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane state="frozen" activePane="bottomLeft" topLeftCell="A10" ySplit="9" xSplit="0"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="3" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="12" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="13" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="13" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="13" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="13" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="13" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="13" width="12.005" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="10">
+        <v>106766</v>
+      </c>
+      <c r="D10" s="10">
+        <v>51548</v>
+      </c>
+      <c r="E10" s="10">
+        <v>55218</v>
+      </c>
+      <c r="F10" s="11">
+        <v>89.1</v>
+      </c>
+      <c r="G10" s="11">
+        <v>88.7</v>
+      </c>
+      <c r="H10" s="11">
+        <v>89.5</v>
+      </c>
+      <c r="I10" s="11">
+        <v>11.9</v>
+      </c>
+      <c r="J10" s="11">
+        <v>11.8</v>
+      </c>
+      <c r="K10" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="10">
+        <v>84163</v>
+      </c>
+      <c r="D11" s="10">
+        <v>40386</v>
+      </c>
+      <c r="E11" s="10">
+        <v>43777</v>
+      </c>
+      <c r="F11" s="11">
+        <v>88.1</v>
+      </c>
+      <c r="G11" s="11">
+        <v>87.7</v>
+      </c>
+      <c r="H11" s="11">
+        <v>88.5</v>
+      </c>
+      <c r="I11" s="11">
+        <v>11.6</v>
+      </c>
+      <c r="J11" s="11">
+        <v>11.5</v>
+      </c>
+      <c r="K11" s="11">
+        <v>11.7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="10">
+        <v>22553</v>
+      </c>
+      <c r="D12" s="10">
+        <v>11137</v>
+      </c>
+      <c r="E12" s="10">
+        <v>11416</v>
+      </c>
+      <c r="F12" s="11">
+        <v>92.9</v>
+      </c>
+      <c r="G12" s="11">
+        <v>92.2</v>
+      </c>
+      <c r="H12" s="11">
+        <v>93.5</v>
+      </c>
+      <c r="I12" s="11">
+        <v>13</v>
+      </c>
+      <c r="J12" s="11">
+        <v>12.8</v>
+      </c>
+      <c r="K12" s="11">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="10">
+        <v>50</v>
+      </c>
+      <c r="D13" s="10">
+        <v>25</v>
+      </c>
+      <c r="E13" s="10">
+        <v>25</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="11">
+        <v>14.1</v>
+      </c>
+      <c r="J13" s="11">
+        <v>13.5</v>
+      </c>
+      <c r="K13" s="11">
+        <v>14.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="I8:K8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:K13"/>
+  <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
       <pane state="frozen" activePane="bottomLeft" topLeftCell="A10" ySplit="9" xSplit="0"/>
     </sheetView>
@@ -1024,7 +1360,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="4"/>
@@ -1132,7 +1468,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -1140,34 +1476,34 @@
         <v>30</v>
       </c>
       <c r="C10" s="10">
-        <v>106766</v>
+        <v>93225</v>
       </c>
       <c r="D10" s="10">
-        <v>51548</v>
+        <v>45800</v>
       </c>
       <c r="E10" s="10">
-        <v>55218</v>
+        <v>47425</v>
       </c>
       <c r="F10" s="11">
-        <v>89.1</v>
+        <v>96.1</v>
       </c>
       <c r="G10" s="11">
-        <v>88.7</v>
+        <v>97.9</v>
       </c>
       <c r="H10" s="11">
-        <v>89.5</v>
+        <v>94.4</v>
       </c>
       <c r="I10" s="11">
-        <v>11.9</v>
+        <v>13.6</v>
       </c>
       <c r="J10" s="11">
-        <v>11.8</v>
+        <v>14.5</v>
       </c>
       <c r="K10" s="11">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+        <v>12.7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1175,34 +1511,34 @@
         <v>31</v>
       </c>
       <c r="C11" s="10">
-        <v>84163</v>
+        <v>72771</v>
       </c>
       <c r="D11" s="10">
-        <v>40386</v>
+        <v>35484</v>
       </c>
       <c r="E11" s="10">
-        <v>43777</v>
+        <v>37287</v>
       </c>
       <c r="F11" s="11">
-        <v>88.1</v>
+        <v>95.7</v>
       </c>
       <c r="G11" s="11">
-        <v>87.7</v>
+        <v>97.6</v>
       </c>
       <c r="H11" s="11">
-        <v>88.5</v>
+        <v>93.8</v>
       </c>
       <c r="I11" s="11">
-        <v>11.6</v>
+        <v>13.3</v>
       </c>
       <c r="J11" s="11">
-        <v>11.5</v>
+        <v>14.3</v>
       </c>
       <c r="K11" s="11">
-        <v>11.7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+        <v>12.4</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -1210,336 +1546,6 @@
         <v>32</v>
       </c>
       <c r="C12" s="10">
-        <v>22553</v>
-      </c>
-      <c r="D12" s="10">
-        <v>11137</v>
-      </c>
-      <c r="E12" s="10">
-        <v>11416</v>
-      </c>
-      <c r="F12" s="11">
-        <v>92.9</v>
-      </c>
-      <c r="G12" s="11">
-        <v>92.2</v>
-      </c>
-      <c r="H12" s="11">
-        <v>93.5</v>
-      </c>
-      <c r="I12" s="11">
-        <v>13</v>
-      </c>
-      <c r="J12" s="11">
-        <v>12.8</v>
-      </c>
-      <c r="K12" s="11">
-        <v>13.1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="10">
-        <v>50</v>
-      </c>
-      <c r="D13" s="10">
-        <v>25</v>
-      </c>
-      <c r="E13" s="10">
-        <v>25</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="I13" s="11">
-        <v>14.1</v>
-      </c>
-      <c r="J13" s="11">
-        <v>13.5</v>
-      </c>
-      <c r="K13" s="11">
-        <v>14.7</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="I8:K8"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:K13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane state="frozen" activePane="bottomLeft" topLeftCell="A10" ySplit="9" xSplit="0"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" style="3" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="13" width="12.005" customWidth="1" bestFit="1"/>
-  </cols>
-  <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="10">
-        <v>93225</v>
-      </c>
-      <c r="D10" s="10">
-        <v>45800</v>
-      </c>
-      <c r="E10" s="10">
-        <v>47425</v>
-      </c>
-      <c r="F10" s="11">
-        <v>96.1</v>
-      </c>
-      <c r="G10" s="11">
-        <v>97.9</v>
-      </c>
-      <c r="H10" s="11">
-        <v>94.4</v>
-      </c>
-      <c r="I10" s="11">
-        <v>13.6</v>
-      </c>
-      <c r="J10" s="11">
-        <v>14.5</v>
-      </c>
-      <c r="K10" s="11">
-        <v>12.7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="10">
-        <v>72771</v>
-      </c>
-      <c r="D11" s="10">
-        <v>35484</v>
-      </c>
-      <c r="E11" s="10">
-        <v>37287</v>
-      </c>
-      <c r="F11" s="11">
-        <v>95.7</v>
-      </c>
-      <c r="G11" s="11">
-        <v>97.6</v>
-      </c>
-      <c r="H11" s="11">
-        <v>93.8</v>
-      </c>
-      <c r="I11" s="11">
-        <v>13.3</v>
-      </c>
-      <c r="J11" s="11">
-        <v>14.3</v>
-      </c>
-      <c r="K11" s="11">
-        <v>12.4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="10">
         <v>20414</v>
       </c>
       <c r="D12" s="10">
@@ -1567,7 +1573,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>

</xml_diff>